<commit_message>
Wrote stuff and stuff
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Bud fate</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>Total shoot appending</t>
   </si>
 </sst>
 </file>
@@ -87,24 +93,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Performance</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -112,6 +100,174 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bud fate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>8.8319999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.112E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1888000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0303E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8350999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8318999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.108671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.138622</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.166654</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25301449999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.28876400000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.33254</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.38053900000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39551500000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.44850600000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.11781</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.031795</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.162738</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.72114299999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Branch shredding</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>7.6800000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.92E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8400000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6800000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.03068E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2288E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4208E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7663999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.121726</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.6079000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.2222999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7983E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.2975000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.4127000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3727000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.9487000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.9455000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21441199999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.14630199999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$4</c:f>
@@ -193,13 +349,180 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shoot appending</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$U$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>0.33215600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92888400000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1545969999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.476769</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1799409999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6515629999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2344689999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.322327</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8126909999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2181899999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8797350000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5714629999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.19008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3455979999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0139800000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.574999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.192540999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.205138000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.316725000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$U$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>0.342524</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95384400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.184933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5424319999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2685827999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7644579999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3711719999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4962770000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1279509999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.5503075000000006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2587380000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0049929999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.6815930000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.8620710000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5995720000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.847175999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.414797999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.699023</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.361192000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="159692672"/>
-        <c:axId val="159703808"/>
+        <c:axId val="76797824"/>
+        <c:axId val="76799360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159692672"/>
+        <c:axId val="76797824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -215,23 +538,26 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Growth cycle</a:t>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> cycle</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159703808"/>
+        <c:crossAx val="76799360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159703808"/>
+        <c:axId val="76799360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -241,7 +567,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -254,21 +580,814 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.3880597014925373E-2"/>
-              <c:y val="0.48408605174353203"/>
-            </c:manualLayout>
-          </c:layout>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159692672"/>
+        <c:crossAx val="76797824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Branch width</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$U$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>7.6800000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.92E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6080000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6800000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9839999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2288E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3823999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7663999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6880000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3023999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8016000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3006999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.6831E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.3358999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4879000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.1007000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.11673500000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.17702200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="141022720"/>
+        <c:axId val="141024640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="141022720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> cycle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141024640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141024640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141022720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Branch shredding</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>7.6800000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.92E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8400000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6800000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.03068E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2288E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4208E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7663999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.121726</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.6079000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.2222999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.7983E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.2975000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.4127000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.3727000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.9487000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.9455000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21441199999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.14630199999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="140760192"/>
+        <c:axId val="141108352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="140760192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> cycle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141108352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141108352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="140760192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bud fate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>8.8319999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.112E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1888000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0303E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8350999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8318999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.108671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.138622</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.166654</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25301449999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.28876400000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.33254</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.38053900000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39551500000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.44850600000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.11781</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.031795</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.162738</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.72114299999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="141209984"/>
+        <c:axId val="141313920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="141209984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> cycle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141313920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141313920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141209984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Voxel addition</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>0.29605999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.791798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9299599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.305507</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9614480000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4941249999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.981031</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.979803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.2328580000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5220830000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3559659999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1344770000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6897339999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.6547900000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1833989999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.387302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.526232</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.7852</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.473932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total shoot appending</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$U$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="1">
+                  <c:v>0.33215600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92888400000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1545969999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.476769</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1799409999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6515629999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2344689999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.322327</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8126909999999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2181899999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8797350000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5714629999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.19008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3455979999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0139800000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.574999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.192540999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.205138000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.316725000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="144373632"/>
+        <c:axId val="144456704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="144373632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> cycle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144456704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="144456704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144373632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -289,20 +1408,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>337858</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>84605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>147358</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>179855</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -312,6 +1431,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>140073</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>128868</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>84044</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5603</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -605,19 +1844,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:U6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -679,7 +1918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -741,7 +1980,7 @@
         <v>0.72114299999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -803,7 +2042,7 @@
         <v>0.14630199999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -865,7 +2104,7 @@
         <v>0.17702200000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -927,7 +2166,7 @@
         <v>16.316725000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1008,66 +2247,215 @@
         <v>17.361192000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>C10-C9</f>
+        <v>3.6096000000000017E-2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:U8" si="1">D10-D9</f>
+        <v>0.13708600000000004</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.22463699999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.17126200000000003</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.21849299999999983</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0.15743799999999997</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.25343799999999983</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0.34252400000000005</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.57983299999999893</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>1.6961069999999996</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.5237690000000006</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>0.43698599999999921</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>0.5003460000000004</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>0.69080799999999964</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>0.83058100000000046</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0.18769799999999925</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>4.6663089999999983</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>2.4199380000000019</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="1"/>
+        <v>1.8427930000000021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>0.29605999999999999</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>0.791798</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>1.9299599999999999</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>2.305507</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>1.9614480000000001</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>1.4941249999999999</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>1.981031</v>
       </c>
-      <c r="J8">
+      <c r="J9">
         <v>2.979803</v>
       </c>
-      <c r="K8">
+      <c r="K9">
         <v>8.2328580000000002</v>
       </c>
-      <c r="L8">
+      <c r="L9">
         <v>7.5220830000000003</v>
       </c>
-      <c r="M8">
+      <c r="M9">
         <v>5.3559659999999996</v>
       </c>
-      <c r="N8">
+      <c r="N9">
         <v>4.1344770000000004</v>
       </c>
-      <c r="O8">
+      <c r="O9">
         <v>4.6897339999999996</v>
       </c>
-      <c r="P8">
+      <c r="P9">
         <v>4.6547900000000002</v>
       </c>
-      <c r="Q8">
+      <c r="Q9">
         <v>7.1833989999999996</v>
       </c>
-      <c r="R8">
+      <c r="R9">
         <v>13.387302</v>
       </c>
-      <c r="S8">
+      <c r="S9">
         <v>13.526232</v>
       </c>
-      <c r="T8">
+      <c r="T9">
         <v>16.7852</v>
       </c>
-      <c r="U8">
+      <c r="U9">
         <v>14.473932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0.33215600000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.92888400000000004</v>
+      </c>
+      <c r="E10">
+        <v>2.1545969999999999</v>
+      </c>
+      <c r="F10">
+        <v>2.476769</v>
+      </c>
+      <c r="G10">
+        <v>2.1799409999999999</v>
+      </c>
+      <c r="H10">
+        <v>1.6515629999999999</v>
+      </c>
+      <c r="I10">
+        <v>2.2344689999999998</v>
+      </c>
+      <c r="J10">
+        <v>3.322327</v>
+      </c>
+      <c r="K10">
+        <v>8.8126909999999992</v>
+      </c>
+      <c r="L10">
+        <v>9.2181899999999999</v>
+      </c>
+      <c r="M10">
+        <v>5.8797350000000002</v>
+      </c>
+      <c r="N10">
+        <v>4.5714629999999996</v>
+      </c>
+      <c r="O10">
+        <v>5.19008</v>
+      </c>
+      <c r="P10">
+        <v>5.3455979999999998</v>
+      </c>
+      <c r="Q10">
+        <v>8.0139800000000001</v>
+      </c>
+      <c r="R10">
+        <v>13.574999999999999</v>
+      </c>
+      <c r="S10">
+        <v>18.192540999999999</v>
+      </c>
+      <c r="T10">
+        <v>19.205138000000002</v>
+      </c>
+      <c r="U10">
+        <v>16.316725000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="V11">
+        <f>SUM(C6:U6)</f>
+        <v>138.33163730000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>